<commit_message>
New test data entry for BITH winter surveys data sheet.
</commit_message>
<xml_diff>
--- a/BITH_winter_survey_data_entry.xlsx
+++ b/BITH_winter_survey_data_entry.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6671" uniqueCount="6615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6679" uniqueCount="6618">
   <si>
     <t>Species</t>
   </si>
@@ -19870,6 +19870,15 @@
   </si>
   <si>
     <t>Starting time (hh:mm) of the fourth survey.</t>
+  </si>
+  <si>
+    <t>PUVI</t>
+  </si>
+  <si>
+    <t>PU-21</t>
+  </si>
+  <si>
+    <t>JDL</t>
   </si>
 </sst>
 </file>
@@ -19941,7 +19950,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -19950,6 +19959,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -20297,10 +20307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20308,8 +20318,8 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="10.83203125" style="5"/>
     <col min="6" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="6" customWidth="1"/>
     <col min="12" max="12" width="16" style="5" customWidth="1"/>
     <col min="13" max="13" width="14.33203125" customWidth="1"/>
   </cols>
@@ -20342,10 +20352,10 @@
       <c r="I1" s="2" t="s">
         <v>6612</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -20356,6 +20366,50 @@
       </c>
       <c r="N1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>6615</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6616</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6617</v>
+      </c>
+      <c r="D2" s="1">
+        <v>26821</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="J2" s="6">
+        <v>15.65443</v>
+      </c>
+      <c r="K2" s="6">
+        <v>27.242439999999998</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -20393,10 +20447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20426,6 +20480,29 @@
       </c>
       <c r="G1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6615</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6616</v>
+      </c>
+      <c r="C2" s="1">
+        <v>26821</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4838</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>